<commit_message>
cambios planificacion y asistencia
</commit_message>
<xml_diff>
--- a/public/uploads/PlanificacioÌn semana 16 2023 (2) (2).xlsx
+++ b/public/uploads/PlanificacioÌn semana 16 2023 (2) (2).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Desktop\planificacion tte8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7555B6DE-0EB6-4577-8BE1-7299273EA081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80AAAD8F-2394-4E93-B6AC-ACE18AF7AEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="829" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2722,6 +2722,34 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="43" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="43" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="43" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="22" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2731,23 +2759,10 @@
     <xf numFmtId="166" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="22" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2763,21 +2778,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="43" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="43" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="43" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2789,6 +2789,42 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="17" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2831,42 +2867,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5698,22 +5698,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
     </row>
     <row r="3" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
@@ -5723,24 +5723,24 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="125"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="130"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="121" t="s">
+      <c r="C6" s="127"/>
+      <c r="D6" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="126"/>
-      <c r="F6" s="127"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -5749,11 +5749,11 @@
       <c r="C7" s="45">
         <v>45033</v>
       </c>
-      <c r="D7" s="111" t="s">
+      <c r="D7" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="112"/>
-      <c r="F7" s="113"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
@@ -5763,11 +5763,11 @@
         <f>C7+1</f>
         <v>45034</v>
       </c>
-      <c r="D8" s="114" t="s">
+      <c r="D8" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="115"/>
-      <c r="F8" s="116"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="120"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
@@ -5777,11 +5777,11 @@
         <f t="shared" ref="C9:C13" si="0">C8+1</f>
         <v>45035</v>
       </c>
-      <c r="D9" s="130" t="s">
+      <c r="D9" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="115"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
@@ -5791,11 +5791,11 @@
         <f t="shared" si="0"/>
         <v>45036</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="115"/>
-      <c r="F10" s="116"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="120"/>
     </row>
     <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
@@ -5844,13 +5844,13 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
     </row>
     <row r="17" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
@@ -5860,50 +5860,50 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="128" t="s">
+      <c r="B18" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="129"/>
+      <c r="C18" s="112"/>
       <c r="D18" s="6">
         <f>'2 TRAFICO'!D4</f>
         <v>34.25655976676385</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="129"/>
+      <c r="C19" s="112"/>
       <c r="D19" s="6" t="str">
         <f>'3 INF.OP'!D4</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="129"/>
+      <c r="C20" s="112"/>
       <c r="D20" s="6">
         <f>'4 MANT.VIAS'!D4</f>
         <v>73.787061994609161</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="129"/>
+      <c r="C21" s="112"/>
       <c r="D21" s="6" t="str">
         <f>'5 INTERFLOW'!D4</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="129"/>
+      <c r="C22" s="112"/>
       <c r="D22" s="6">
         <f>'7 MIES'!D4</f>
         <v>78.187583444592804</v>
@@ -5911,6 +5911,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="B21:C21"/>
@@ -5919,13 +5926,6 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.1811023622047245" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
@@ -7465,11 +7465,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="157"/>
-      <c r="I1" s="158"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
       <c r="J1" s="82">
         <v>14</v>
       </c>
@@ -7493,19 +7493,19 @@
       </c>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="160"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -7523,20 +7523,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="83">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>78.399999999999991</v>
@@ -7567,21 +7567,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="152"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="43">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v>34.25655976676385</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="22">
         <f>IF(J1=0, "", SUM(J9:J13))</f>
         <v>28</v>
@@ -7617,11 +7617,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="142"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="1">IF(J1=0, "", (J4/J3)*100)</f>
         <v>35.714285714285722</v>
@@ -7669,26 +7669,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="160"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -7714,18 +7714,18 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="144"/>
-      <c r="F8" s="146"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="158"/>
       <c r="G8" s="69" t="s">
         <v>137</v>
       </c>
       <c r="H8" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="150"/>
+      <c r="I8" s="162"/>
       <c r="J8" s="70">
         <f>+'0 Control'!$C$7</f>
         <v>45033</v>
@@ -7941,33 +7941,26 @@
       <c r="P13" s="68"/>
     </row>
     <row r="14" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="149" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="138"/>
-      <c r="L14" s="138"/>
-      <c r="M14" s="138"/>
-      <c r="N14" s="138"/>
-      <c r="O14" s="138"/>
-      <c r="P14" s="139"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="150"/>
+      <c r="H14" s="150"/>
+      <c r="I14" s="150"/>
+      <c r="J14" s="150"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="150"/>
+      <c r="M14" s="150"/>
+      <c r="N14" s="150"/>
+      <c r="O14" s="150"/>
+      <c r="P14" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B14:P14"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -7977,6 +7970,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I12">
     <cfRule type="expression" dxfId="206" priority="24">
@@ -8150,11 +8150,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="157"/>
-      <c r="I1" s="158"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
       <c r="J1" s="34">
         <v>6</v>
       </c>
@@ -8178,19 +8178,19 @@
       </c>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="160"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="158"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -8208,20 +8208,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>33.599999999999994</v>
@@ -8252,21 +8252,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="152"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="43" t="str">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v/>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J45))</f>
         <v>0</v>
@@ -8302,11 +8302,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="142"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>0</v>
@@ -8354,26 +8354,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="160"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -9382,13 +9382,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B46:P46"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -9398,6 +9391,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I36 K10:M36">
     <cfRule type="expression" dxfId="169" priority="12">
@@ -9575,11 +9575,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="15"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
       <c r="J1" s="34">
         <v>21</v>
       </c>
@@ -9602,19 +9602,19 @@
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="159"/>
+      <c r="C2" s="145"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -9633,20 +9633,20 @@
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="161"/>
+      <c r="C3" s="147"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>117.6</v>
@@ -9678,21 +9678,21 @@
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="151"/>
+      <c r="C4" s="137"/>
       <c r="D4" s="43">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v>73.787061994609161</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J69))</f>
         <v>122</v>
@@ -9729,11 +9729,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>103.74149659863947</v>
@@ -9783,26 +9783,26 @@
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="147"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="159"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -9829,18 +9829,18 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
-      <c r="B8" s="143"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="145"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="157"/>
       <c r="G8" s="44" t="s">
         <v>137</v>
       </c>
       <c r="H8" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="149"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="26">
         <f>+'0 Control'!$C$7</f>
         <v>45033</v>
@@ -11458,13 +11458,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B70:P70"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -11474,6 +11467,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I70:I233">
     <cfRule type="cellIs" dxfId="138" priority="119" operator="equal">
@@ -11614,11 +11614,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="157"/>
-      <c r="I1" s="158"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
       <c r="J1" s="34">
         <v>1</v>
       </c>
@@ -11638,19 +11638,19 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="160"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="158"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -11668,20 +11668,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>5.6</v>
@@ -11712,21 +11712,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="152"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="43" t="str">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v/>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J16))</f>
         <v>0</v>
@@ -11762,11 +11762,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="142"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>0</v>
@@ -11814,26 +11814,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="160"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -12071,7 +12071,7 @@
       <c r="P16" s="32"/>
     </row>
     <row r="17" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="137" t="s">
+      <c r="B17" s="149" t="s">
         <v>141</v>
       </c>
       <c r="C17" s="169"/>
@@ -12091,6 +12091,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B17:P17"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -12100,13 +12107,6 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I17:I180">
     <cfRule type="cellIs" dxfId="112" priority="150" operator="equal">
@@ -12221,11 +12221,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
       <c r="J1" s="34">
         <v>41</v>
       </c>
@@ -12245,19 +12245,19 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="159"/>
+      <c r="C2" s="145"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -12275,20 +12275,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="161"/>
+      <c r="C3" s="147"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>229.6</v>
@@ -12319,21 +12319,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="151"/>
+      <c r="C4" s="137"/>
       <c r="D4" s="43">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v>78.187583444592804</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J103))</f>
         <v>189</v>
@@ -12369,11 +12369,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>82.317073170731717</v>
@@ -12421,26 +12421,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="147"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="159"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -12466,18 +12466,18 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="143"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="145"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="157"/>
       <c r="G8" s="56" t="s">
         <v>137</v>
       </c>
       <c r="H8" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="149"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="26">
         <f>+'0 Control'!$C$7</f>
         <v>45033</v>
@@ -14933,7 +14933,7 @@
       <c r="P103" s="32"/>
     </row>
     <row r="104" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="137"/>
+      <c r="A104" s="149"/>
       <c r="B104" s="171"/>
       <c r="C104" s="171"/>
       <c r="D104" s="171"/>
@@ -14951,13 +14951,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
     <mergeCell ref="A104:O104"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -14967,6 +14960,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="H104">
     <cfRule type="cellIs" dxfId="95" priority="665" operator="equal">
@@ -15229,11 +15229,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="157"/>
-      <c r="I1" s="158"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
       <c r="J1" s="34">
         <v>1</v>
       </c>
@@ -15253,19 +15253,19 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="160"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="158"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -15283,20 +15283,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>5.6</v>
@@ -15327,21 +15327,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="152"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="43" t="str">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v/>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J17))</f>
         <v>0</v>
@@ -15377,11 +15377,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="142"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>0</v>
@@ -15429,26 +15429,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="160"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -15682,7 +15682,7 @@
       <c r="P17" s="32"/>
     </row>
     <row r="18" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="149" t="s">
         <v>141</v>
       </c>
       <c r="C18" s="169"/>
@@ -15702,13 +15702,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B18:P18"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -15718,6 +15711,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I181">
     <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
@@ -15836,11 +15836,11 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="157"/>
-      <c r="I1" s="158"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
       <c r="J1" s="34">
         <v>1</v>
       </c>
@@ -15860,19 +15860,19 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="145" t="str">
         <f>'0 Control'!B5:F5</f>
         <v>SEMANA 16</v>
       </c>
-      <c r="C2" s="160"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="158"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="66" t="s">
         <v>23</v>
       </c>
@@ -15890,20 +15890,20 @@
       <c r="P2" s="81"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="162"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="42">
         <v>5.6</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="21">
         <f t="shared" ref="J3:P3" si="0">IF(J1=0, "", $D$3*J1)</f>
         <v>5.6</v>
@@ -15934,21 +15934,21 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="152"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="43" t="str">
         <f>IF((SUM(J4:P4)/SUM(J3:P3))*100=0, "", (SUM(J4:P4)/SUM(J3:P3))*100)</f>
         <v/>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="153" t="s">
+      <c r="G4" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="154"/>
-      <c r="I4" s="155"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="22">
         <f t="shared" ref="J4:P4" si="1">IF(J1=0, "", SUM(J9:J30))</f>
         <v>0</v>
@@ -15984,11 +15984,11 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="142"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="154"/>
       <c r="J5" s="33">
         <f t="shared" ref="J5:P5" si="2">IF(J1=0, "", (J4/J3)*100)</f>
         <v>0</v>
@@ -16036,26 +16036,26 @@
       <c r="P6" s="40"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="155" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="155" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="155" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="149" t="s">
+      <c r="H7" s="160"/>
+      <c r="I7" s="161" t="s">
         <v>129</v>
       </c>
       <c r="J7" s="24" t="s">
@@ -16553,7 +16553,7 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="137" t="s">
+      <c r="B31" s="149" t="s">
         <v>141</v>
       </c>
       <c r="C31" s="169"/>
@@ -16573,6 +16573,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B31:P31"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B7:B8"/>
@@ -16582,13 +16589,6 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I194">
     <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
@@ -16685,39 +16685,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="13292f55-de52-430d-b14b-7bbbc007da08">
-      <UserInfo>
-        <DisplayName>Lizana Fuentes Carolina Nazarena (Codelco-Teniente)</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Toro Uribe Daniza (Codelco-Teniente)</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Osorio Pavéz Adriana Isabel  (Codelco-Teniente)</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Nuñez Segulla Christian Andres (Codelco-Teniente)</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd65d8d-9a0c-413b-b337-26d3d6865661">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="13292f55-de52-430d-b14b-7bbbc007da08" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010077EEB9F3B60CE24689AC59713F949007" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9dd14038330b71dbed40bf1cfe646435">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cd65d8d-9a0c-413b-b337-26d3d6865661" xmlns:ns3="13292f55-de52-430d-b14b-7bbbc007da08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f683da081425f6d2a484969eabc83748" ns2:_="" ns3:_="">
     <xsd:import namespace="0cd65d8d-9a0c-413b-b337-26d3d6865661"/>
@@ -16940,6 +16907,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="13292f55-de52-430d-b14b-7bbbc007da08">
+      <UserInfo>
+        <DisplayName>Lizana Fuentes Carolina Nazarena (Codelco-Teniente)</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Toro Uribe Daniza (Codelco-Teniente)</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Osorio Pavéz Adriana Isabel  (Codelco-Teniente)</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Nuñez Segulla Christian Andres (Codelco-Teniente)</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd65d8d-9a0c-413b-b337-26d3d6865661">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="13292f55-de52-430d-b14b-7bbbc007da08" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6694C59C-A506-40B5-9FBF-5C26D4C67255}">
   <ds:schemaRefs>
@@ -16949,17 +16949,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE985242-E434-4BC2-931D-7A535FD5A5E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="13292f55-de52-430d-b14b-7bbbc007da08"/>
-    <ds:schemaRef ds:uri="0cd65d8d-9a0c-413b-b337-26d3d6865661"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F428DB-A42C-4360-AF24-07D2BED7F7E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16976,4 +16965,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE985242-E434-4BC2-931D-7A535FD5A5E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="13292f55-de52-430d-b14b-7bbbc007da08"/>
+    <ds:schemaRef ds:uri="0cd65d8d-9a0c-413b-b337-26d3d6865661"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>